<commit_message>
added stuff about git
</commit_message>
<xml_diff>
--- a/Tables/data_sheet.xlsx
+++ b/Tables/data_sheet.xlsx
@@ -2,20 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshellswell/Physics/My_Work/Major_Project_Report/Tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06251412-9F4E-FB49-9818-C67F29C29A22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E24EDD5F-F2E0-0549-B823-3501EB818F4E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7080" yWindow="2440" windowWidth="17900" windowHeight="13480" xr2:uid="{9EA72C83-D489-924F-8AE4-A6DE8AC8E362}"/>
+    <workbookView xWindow="7080" yWindow="2440" windowWidth="17900" windowHeight="13480" activeTab="1" xr2:uid="{9EA72C83-D489-924F-8AE4-A6DE8AC8E362}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Excel2LaTeX" sheetId="2" state="hidden" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="58">
   <si>
     <t>Cons</t>
   </si>
@@ -163,6 +164,42 @@
   </si>
   <si>
     <t>[   64.83177713 -1452.6296242  16378.18197628]</t>
+  </si>
+  <si>
+    <t>Old a</t>
+  </si>
+  <si>
+    <t>Old b</t>
+  </si>
+  <si>
+    <t>Old c</t>
+  </si>
+  <si>
+    <t>New a</t>
+  </si>
+  <si>
+    <t>New b</t>
+  </si>
+  <si>
+    <t>New c</t>
+  </si>
+  <si>
+    <t>RangeAddress</t>
+  </si>
+  <si>
+    <t>Options</t>
+  </si>
+  <si>
+    <t>CellWidth</t>
+  </si>
+  <si>
+    <t>Indent</t>
+  </si>
+  <si>
+    <t>FileName</t>
+  </si>
+  <si>
+    <t>Sheet1.tex</t>
   </si>
 </sst>
 </file>
@@ -217,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -232,6 +269,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,19 +586,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CA1BEE-0046-0245-B107-5C71B81A858B}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <f>COUNT(Sheet1!$A$20:$G$32)</f>
+        <v>72</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE71CC1C-B8D0-5A4F-A1F1-3E30FDAD1CFF}">
-  <dimension ref="A1:I16"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.1640625" customWidth="1"/>
     <col min="8" max="8" width="61.1640625" customWidth="1"/>
     <col min="9" max="9" width="63.1640625" customWidth="1"/>
@@ -935,6 +1027,305 @@
         <v>43</v>
       </c>
     </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="11">
+        <v>-2.74305331E-4</v>
+      </c>
+      <c r="C21" s="12">
+        <v>3.9684121600000002</v>
+      </c>
+      <c r="D21" s="12">
+        <v>57.173957999999999</v>
+      </c>
+      <c r="E21" s="10">
+        <v>-3.8307972500000002E-17</v>
+      </c>
+      <c r="F21" s="12">
+        <v>4</v>
+      </c>
+      <c r="G21" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" s="10">
+        <v>2.1877466400000001E-4</v>
+      </c>
+      <c r="C22" s="12">
+        <v>5.5008272900000001</v>
+      </c>
+      <c r="D22" s="12">
+        <v>6.3010920700000002</v>
+      </c>
+      <c r="E22" s="10">
+        <v>-3.8307972500000002E-17</v>
+      </c>
+      <c r="F22" s="12">
+        <v>4</v>
+      </c>
+      <c r="G22" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="8">
+        <v>18.650903719999999</v>
+      </c>
+      <c r="C23">
+        <v>-333.56881528999997</v>
+      </c>
+      <c r="D23">
+        <v>1919.7929012100001</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1.6129672599999999E-17</v>
+      </c>
+      <c r="F23" s="12">
+        <v>12</v>
+      </c>
+      <c r="G23" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="10">
+        <v>4</v>
+      </c>
+      <c r="C24" s="12">
+        <v>2</v>
+      </c>
+      <c r="D24" s="12">
+        <v>2.4073590000000002E-12</v>
+      </c>
+      <c r="E24" s="10">
+        <v>4.0324181499999997E-18</v>
+      </c>
+      <c r="F24" s="12">
+        <v>3</v>
+      </c>
+      <c r="G24" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="10">
+        <v>-1.93556071E-16</v>
+      </c>
+      <c r="C25" s="12">
+        <v>42</v>
+      </c>
+      <c r="D25" s="12">
+        <v>-5.7204570300000002E-13</v>
+      </c>
+      <c r="E25" s="10">
+        <v>4.0324181499999997E-18</v>
+      </c>
+      <c r="F25" s="12">
+        <v>3</v>
+      </c>
+      <c r="G25" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="4">
+        <v>64.831777130000006</v>
+      </c>
+      <c r="C26">
+        <v>-1452.6296242000001</v>
+      </c>
+      <c r="D26">
+        <v>16378.181976280001</v>
+      </c>
+      <c r="E26" s="13">
+        <v>4.8389017900000002E-17</v>
+      </c>
+      <c r="F26" s="12">
+        <v>22</v>
+      </c>
+      <c r="G26" s="12">
+        <v>-9.5340950500000003E-14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="10">
+        <v>-6.4518690499999998E-17</v>
+      </c>
+      <c r="C27" s="12">
+        <v>34</v>
+      </c>
+      <c r="D27" s="12">
+        <v>-1.9068190100000001E-13</v>
+      </c>
+      <c r="E27" s="10">
+        <v>-8.0648363099999994E-18</v>
+      </c>
+      <c r="F27" s="12">
+        <v>10</v>
+      </c>
+      <c r="G27" s="12">
+        <v>-4.7670475200000003E-14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" s="10">
+        <v>-1.93556071E-16</v>
+      </c>
+      <c r="C28" s="12">
+        <v>34</v>
+      </c>
+      <c r="D28" s="12">
+        <v>-1.9068190100000001E-13</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1.6129672599999999E-17</v>
+      </c>
+      <c r="F28" s="12">
+        <v>12</v>
+      </c>
+      <c r="G28" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="8">
+        <v>0.39682347000000001</v>
+      </c>
+      <c r="C29">
+        <v>7.1301155700000001</v>
+      </c>
+      <c r="D29">
+        <v>7.42466252</v>
+      </c>
+      <c r="E29" s="10">
+        <v>-4.0324181499999999E-17</v>
+      </c>
+      <c r="F29" s="12">
+        <v>6</v>
+      </c>
+      <c r="G29" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="8">
+        <v>10.821549259999999</v>
+      </c>
+      <c r="C30">
+        <v>-356.63291243999998</v>
+      </c>
+      <c r="D30">
+        <v>8557.2491950799995</v>
+      </c>
+      <c r="E30" s="10">
+        <v>20</v>
+      </c>
+      <c r="F30" s="12">
+        <v>220</v>
+      </c>
+      <c r="G30" s="12">
+        <v>1.9830917700000001E-11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="8">
+        <v>7.0177650800000002</v>
+      </c>
+      <c r="C31">
+        <v>304.87460374</v>
+      </c>
+      <c r="D31">
+        <v>4899.1962252900003</v>
+      </c>
+      <c r="E31" s="10">
+        <v>-1.6129672599999999E-17</v>
+      </c>
+      <c r="F31" s="12">
+        <v>20</v>
+      </c>
+      <c r="G31" s="12">
+        <v>-9.5340950500000003E-14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="8">
+        <v>0.27241768999999999</v>
+      </c>
+      <c r="C32">
+        <v>4.5819117499999997</v>
+      </c>
+      <c r="D32">
+        <v>8.3367521100000008</v>
+      </c>
+      <c r="E32" s="10">
+        <v>-3.8307972500000002E-17</v>
+      </c>
+      <c r="F32" s="12">
+        <v>4</v>
+      </c>
+      <c r="G32" s="12">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>